<commit_message>
adding more data to excel files
</commit_message>
<xml_diff>
--- a/main/runs.xlsx
+++ b/main/runs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jagde\Desktop\Jujhaar\programming\my programmes\python\tkinter\cricket-scores\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E16FFB-FB35-4020-B31B-0293657393C4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779AAC97-CF3A-4753-9C9B-78A17C65A4E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5847D5F8-8787-437A-ADF0-41891A15A347}"/>
+    <workbookView xWindow="1548" yWindow="348" windowWidth="15576" windowHeight="12216" xr2:uid="{5847D5F8-8787-437A-ADF0-41891A15A347}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>RUNS</t>
   </si>
@@ -69,6 +69,27 @@
   </si>
   <si>
     <t>SRH</t>
+  </si>
+  <si>
+    <t>WATSON</t>
+  </si>
+  <si>
+    <t>SMITH</t>
+  </si>
+  <si>
+    <t>GAYLE</t>
+  </si>
+  <si>
+    <t>SACHIN</t>
+  </si>
+  <si>
+    <t>DRAVID</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>DC</t>
   </si>
 </sst>
 </file>
@@ -420,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E947901E-E577-48FB-B7FB-051BBD2936BB}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E2" sqref="E2:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,17 +474,17 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>110</v>
+        <v>693</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <f>ROUNDDOWN(B2/D2,2)</f>
-        <v>36.659999999999997</v>
+        <v>69.3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -471,17 +492,17 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>85</v>
+        <v>385</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <f>ROUNDDOWN(B3/D3,2)</f>
-        <v>28.33</v>
+        <f t="shared" ref="E3:E10" si="0">ROUNDDOWN(B3/D3,2)</f>
+        <v>38.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -489,17 +510,17 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>78</v>
+        <v>578</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E4">
-        <f>ROUNDDOWN(B4/D4,2)</f>
-        <v>26</v>
+        <f t="shared" si="0"/>
+        <v>57.8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -507,17 +528,107 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>59</v>
+        <v>473</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E5">
-        <f>ROUNDDOWN(B5/D5,2)</f>
-        <v>19.66</v>
+        <f t="shared" si="0"/>
+        <v>47.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>398</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>39.799999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>659</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>65.900000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>603</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>60.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>690</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>573</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>57.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>